<commit_message>
add: add deflecton plot (still error)
</commit_message>
<xml_diff>
--- a/excel/beam-analysis.xlsx
+++ b/excel/beam-analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Danar_diskG\FRONTEND DEVELOPMENT\JAVASCRIPT\project\clt-technical-test\javascript-test\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C979770-CC2E-494B-9B26-E29D0A54E99A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2533D53-4B1C-46F9-93A3-07E0D747A6DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2760" yWindow="6804" windowWidth="26844" windowHeight="15936" activeTab="1" xr2:uid="{06323F42-374D-8043-B3CD-A4C25C676AC9}"/>
   </bookViews>
@@ -4210,15 +4210,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>158115</xdr:colOff>
+      <xdr:colOff>160020</xdr:colOff>
       <xdr:row>110</xdr:row>
-      <xdr:rowOff>128905</xdr:rowOff>
+      <xdr:rowOff>132715</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
+      <xdr:colOff>179070</xdr:colOff>
       <xdr:row>116</xdr:row>
-      <xdr:rowOff>27940</xdr:rowOff>
+      <xdr:rowOff>26035</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4233,8 +4233,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5682615" y="21083905"/>
-          <a:ext cx="28750260" cy="1042035"/>
+          <a:off x="2827020" y="21735415"/>
+          <a:ext cx="12763500" cy="960120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6566,15 +6566,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>43180</xdr:colOff>
+      <xdr:colOff>169455</xdr:colOff>
       <xdr:row>132</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>46265</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>149</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>452030</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>162198</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -6591,8 +6591,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="22395180" y="25260300"/>
-          <a:ext cx="3782695" cy="3171825"/>
+          <a:off x="21532669" y="28662086"/>
+          <a:ext cx="4024540" cy="4170862"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -7530,10 +7530,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>97155</xdr:colOff>
       <xdr:row>146</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>20955</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5690779" cy="490764"/>
     <xdr:pic>
@@ -7557,7 +7557,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10563225" y="27822525"/>
+          <a:off x="11064512" y="32256276"/>
           <a:ext cx="5690779" cy="490764"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7573,10 +7573,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>121376</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>422638</xdr:colOff>
       <xdr:row>148</xdr:row>
-      <xdr:rowOff>88719</xdr:rowOff>
+      <xdr:rowOff>65315</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="7040335" cy="741136"/>
     <xdr:pic>
@@ -7600,7 +7600,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12476662" y="32759469"/>
+          <a:off x="11852638" y="32736065"/>
           <a:ext cx="7040335" cy="741136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7617,9 +7617,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>124460</xdr:colOff>
-      <xdr:row>149</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>252640</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>162198</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1099276" cy="560614"/>
     <xdr:pic>
@@ -7643,7 +7643,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="21777960" y="28432125"/>
+          <a:off x="20867461" y="32832948"/>
           <a:ext cx="1099276" cy="560614"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8495,8 +8495,8 @@
   </sheetPr>
   <dimension ref="A1:AB1003"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O89" sqref="O89"/>
+    <sheetView showGridLines="0" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J127" sqref="J127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -16357,8 +16357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894285D5-4F9B-484A-90B9-FBDD72A96AD5}">
   <dimension ref="A1:AJ347"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AC78" sqref="AC78"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R114" sqref="R114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13.8"/>

</xml_diff>